<commit_message>
Deprecated Peppol AS2 v1 - TICC-123
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Transport profiles v7.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Transport profiles v7.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="110" windowWidth="18920" windowHeight="12300"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="18915" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Transport Profile" sheetId="5" r:id="rId1"/>
@@ -583,18 +583,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7265625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.453125" style="7"/>
+    <col min="5" max="5" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1">
@@ -652,7 +652,11 @@
         <v>3</v>
       </c>
       <c r="E3" s="3" t="b">
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6">

</xml_diff>